<commit_message>
added bzhang data analysis
</commit_message>
<xml_diff>
--- a/Given_Data/NBA_financial_data.xlsx
+++ b/Given_Data/NBA_financial_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amedeloitte.sharepoint.com/sites/UMDAnalyticsConsortium/Shared Documents/Datathon/Spring 2024/Datathon Materials/Data Files/2024_datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bzhang/Desktop/UMD/Datathon2024/Given_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{1C3B10AD-5469-4715-9304-5C68EC0BDA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBD79D9A-9570-4AC8-889E-B0FEAFE6B57B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E966FA40-F9A6-D040-81DC-813E891A0D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29370" yWindow="-2700" windowWidth="29655" windowHeight="19320" activeTab="1" xr2:uid="{5527E2D9-5069-4370-96BE-353886BA1CD4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{5527E2D9-5069-4370-96BE-353886BA1CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="159">
   <si>
     <t>City</t>
   </si>
@@ -210,9 +210,6 @@
     <t>United Wholesale Mortgage</t>
   </si>
   <si>
-    <t>San Franciso</t>
-  </si>
-  <si>
     <t>California</t>
   </si>
   <si>
@@ -237,20 +234,6 @@
     <t>Credit Karma</t>
   </si>
   <si>
-    <r>
-      <t>Indianapolis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>Indiana</t>
   </si>
   <si>
@@ -522,6 +505,15 @@
   </si>
   <si>
     <t>The revenue generated from ticket sales by the team during the 2019/2020 season in millions of US dollars.</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Minneapolis</t>
+  </si>
+  <si>
+    <t>Indianapolis</t>
   </si>
 </sst>
 </file>
@@ -689,9 +681,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -729,7 +721,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -835,7 +827,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -977,7 +969,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,26 +979,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C07E2A1-0DDC-40FF-ACB8-1A23FE8E1004}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="1"/>
+    <col min="12" max="12" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1082,7 +1075,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1120,7 +1113,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1158,7 +1151,7 @@
         <v>55.1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1196,7 +1189,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1234,7 +1227,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -1272,7 +1265,7 @@
         <v>67.400000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
@@ -1310,7 +1303,7 @@
         <v>57.4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
@@ -1348,7 +1341,7 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>52</v>
       </c>
@@ -1386,18 +1379,18 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="E11" s="3">
         <v>1400</v>
@@ -1409,7 +1402,7 @@
         <v>18064</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" s="8">
         <v>765</v>
@@ -1424,18 +1417,18 @@
         <v>100.4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="E12" s="3">
         <v>235</v>
@@ -1447,7 +1440,7 @@
         <v>18055</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I12" s="8">
         <v>381</v>
@@ -1462,18 +1455,18 @@
         <v>66.599999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="E13" s="3">
         <v>183</v>
@@ -1485,7 +1478,7 @@
         <v>17923</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I13" s="8">
         <v>263</v>
@@ -1500,18 +1493,18 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="E14" s="3">
         <v>375</v>
@@ -1523,7 +1516,7 @@
         <v>19068</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I14" s="8">
         <v>425</v>
@@ -1538,18 +1531,18 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="E15" s="3">
         <v>375</v>
@@ -1561,7 +1554,7 @@
         <v>18997</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I15" s="8">
         <v>516</v>
@@ -1576,18 +1569,18 @@
         <v>116.8</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="E16" s="3">
         <v>250</v>
@@ -1599,7 +1592,7 @@
         <v>17794</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I16" s="8">
         <v>258</v>
@@ -1614,18 +1607,18 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="E17" s="3">
         <v>213</v>
@@ -1637,7 +1630,7 @@
         <v>19600</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I17" s="8">
         <v>371</v>
@@ -1652,18 +1645,18 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E18" s="3">
         <v>1200</v>
@@ -1690,18 +1683,18 @@
         <v>46.9</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="E19" s="3">
         <v>104</v>
@@ -1713,7 +1706,7 @@
         <v>18978</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I19" s="8">
         <v>259</v>
@@ -1728,18 +1721,18 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="E20" s="3">
         <v>114</v>
@@ -1766,7 +1759,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -1774,10 +1767,10 @@
         <v>23</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="3">
         <v>123</v>
@@ -1789,7 +1782,7 @@
         <v>19812</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I21" s="8">
         <v>504</v>
@@ -1804,18 +1797,18 @@
         <v>109.1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E22" s="3">
         <v>89.2</v>
@@ -1827,7 +1820,7 @@
         <v>18203</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I22" s="8">
         <v>267</v>
@@ -1842,18 +1835,18 @@
         <v>52.2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E23" s="3">
         <v>480</v>
@@ -1865,7 +1858,7 @@
         <v>18846</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I23" s="8">
         <v>261</v>
@@ -1880,18 +1873,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="D24" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="E24" s="3">
         <v>210</v>
@@ -1903,7 +1896,7 @@
         <v>20478</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I24" s="8">
         <v>371</v>
@@ -1918,18 +1911,18 @@
         <v>58.7</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="E25" s="3">
         <v>89</v>
@@ -1941,7 +1934,7 @@
         <v>17071</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I25" s="8">
         <v>366</v>
@@ -1956,18 +1949,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="E26" s="3">
         <v>262</v>
@@ -1979,7 +1972,7 @@
         <v>19441</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I26" s="8">
         <v>300</v>
@@ -1994,18 +1987,18 @@
         <v>52.8</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="E27" s="3">
         <v>558.20000000000005</v>
@@ -2017,7 +2010,7 @@
         <v>17583</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I27" s="8">
         <v>289</v>
@@ -2032,18 +2025,18 @@
         <v>56.1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E28" s="3">
         <v>186</v>
@@ -2055,7 +2048,7 @@
         <v>18418</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I28" s="8">
         <v>319</v>
@@ -2070,18 +2063,18 @@
         <v>56.3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="E29" s="3">
         <v>288</v>
@@ -2093,7 +2086,7 @@
         <v>19800</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I29" s="8">
         <v>305</v>
@@ -2108,18 +2101,18 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="E30" s="2">
         <v>93</v>
@@ -2131,7 +2124,7 @@
         <v>18306</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I30" s="9">
         <v>274</v>
@@ -2146,18 +2139,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="E31" s="7">
         <v>260</v>
@@ -2169,7 +2162,7 @@
         <v>20356</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I31" s="9">
         <v>323</v>
@@ -2184,10 +2177,10 @@
         <v>60.9</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="12:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="12:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L33" s="4"/>
     </row>
   </sheetData>
@@ -2200,118 +2193,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4B32E6-C0AB-4E19-B0BD-C85F3C3EA205}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2320,6 +2313,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005839CC2DBF3E7D449D1071A3660AD348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6532814d65e65a30435dc4676eac13bd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="59e007f7-2ec2-4ce4-ac02-a8e8f8339950" xmlns:ns3="f2ee048e-e823-4989-b592-6f5027b51d7a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb05717631d668bfea540b4f11d44fed" ns2:_="" ns3:_="">
     <xsd:import namespace="59e007f7-2ec2-4ce4-ac02-a8e8f8339950"/>
@@ -2522,22 +2530,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C620FC2-5529-48A4-80B9-FBB878C210D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{646F3588-AD96-45B0-BF11-970C3451F814}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="f2ee048e-e823-4989-b592-6f5027b51d7a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="59e007f7-2ec2-4ce4-ac02-a8e8f8339950"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05B8CAD8-67BF-4BD6-BFB1-49F3855AE613}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2554,29 +2572,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C620FC2-5529-48A4-80B9-FBB878C210D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{646F3588-AD96-45B0-BF11-970C3451F814}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f2ee048e-e823-4989-b592-6f5027b51d7a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="59e007f7-2ec2-4ce4-ac02-a8e8f8339950"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>